<commit_message>
inserted effort table names and headers
</commit_message>
<xml_diff>
--- a/Effort.xlsx
+++ b/Effort.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tobia\dev\database_proj_group_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D630A83A-0601-4780-91E0-B2C87F7E5FD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8FE9141-7512-49C4-95B4-DBDF2D2463FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F7E54E07-7039-4460-BFB6-29BB1B2389A3}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{F7E54E07-7039-4460-BFB6-29BB1B2389A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -22,6 +22,59 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Group number</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>1. Conceptual Design</t>
+  </si>
+  <si>
+    <t>2. Logical Design</t>
+  </si>
+  <si>
+    <t>3. Implementation</t>
+  </si>
+  <si>
+    <t>4. Database Instance</t>
+  </si>
+  <si>
+    <t>5. SQL Table Modifications</t>
+  </si>
+  <si>
+    <t>6. SQL Data Queries</t>
+  </si>
+  <si>
+    <t>7. SQL Programming</t>
+  </si>
+  <si>
+    <t>8. Java Database Access</t>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+  </si>
+  <si>
+    <t>Bjarne Larsen</t>
+  </si>
+  <si>
+    <t>Marcus Lemser</t>
+  </si>
+  <si>
+    <t>Maximillian Mortesen</t>
+  </si>
+  <si>
+    <t>Oscar Bjerregaard</t>
+  </si>
+  <si>
+    <t>Tobias Frederiksen</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -371,14 +424,88 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BFE92ED-15D2-4E70-A584-1706FF92188D}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:K6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>